<commit_message>
added link to github flow text
</commit_message>
<xml_diff>
--- a/Docs/ChexmanPR.xlsx
+++ b/Docs/ChexmanPR.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Shared folders\Windows\Shared Documents\Collective\Site\Chexman\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCC401C-06EA-419E-AE6C-8D90E8D6D499}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{394E4A90-1461-4B89-A170-C28BC596CAB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7590" yWindow="3180" windowWidth="18300" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="85">
   <si>
     <t>Inception</t>
   </si>
@@ -274,13 +274,16 @@
     <t>Define branching strategy</t>
   </si>
   <si>
-    <t>Based on github-flow but simpler</t>
-  </si>
-  <si>
     <t>Maria</t>
   </si>
   <si>
     <t>E1S5</t>
+  </si>
+  <si>
+    <t>https://quangnguyennd.medium.com/git-flow-vs-github-flow-620c922b2cbd</t>
+  </si>
+  <si>
+    <t>Based on github-flow</t>
   </si>
 </sst>
 </file>
@@ -849,7 +852,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,22 +977,25 @@
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>80</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D6" t="s">
         <v>57</v>
       </c>
       <c r="E6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F6" s="2">
         <v>44527</v>
+      </c>
+      <c r="H6" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>